<commit_message>
update footer & animation
</commit_message>
<xml_diff>
--- a/doc/14th-IICCwebsite.xlsx
+++ b/doc/14th-IICCwebsite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\You-Chia\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\You-Chia\Dropbox\IICC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
   <si>
     <t>競賽資訊</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,10 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>友站連結</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>照片與影片</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,263 +118,258 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>English</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作團隊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>複賽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>決賽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本屆題目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>複賽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>決賽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一屆</t>
+  </si>
+  <si>
+    <t>歷屆資訊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二屆</t>
+  </si>
+  <si>
+    <t>第三屆</t>
+  </si>
+  <si>
+    <t>第六屆</t>
+  </si>
+  <si>
+    <t>第七屆</t>
+  </si>
+  <si>
+    <t>第九屆</t>
+  </si>
+  <si>
+    <t>第十屆</t>
+  </si>
+  <si>
+    <t>第十一屆</t>
+  </si>
+  <si>
+    <t>第十二屆</t>
+  </si>
+  <si>
+    <t>第十三屆</t>
+  </si>
+  <si>
+    <t>關於競賽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>留言板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>媒體報導</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>網站架構</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>複賽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOME&amp;NEWS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>協辦單位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贊助單位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意事項</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>報名資訊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教師研習營</t>
+  </si>
+  <si>
+    <t>學校推廣說明會</t>
+  </si>
+  <si>
+    <t>官方說明會</t>
+  </si>
+  <si>
+    <t>相關活動</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>培訓計畫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>時間與場地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一梯初賽晉級名單</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大事紀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>競賽歷史</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>競賽理念</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二梯初賽晉級名單</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文宣品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>電子報</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q&amp;A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常見問題</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>點我進入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常用表格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初賽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>辦法與繳費</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>報名流程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>組隊辦法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>緣起</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>競賽介紹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>組隊辦法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>報名網站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常用表格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大會獎項</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>複賽企業獎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>決賽企業獎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初賽時程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>複賽晉級名單</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第五屆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第八屆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>留言板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第四屆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>最新消息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>留言板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(自動往下)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>English</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工作團隊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>複賽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>決賽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本屆題目</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>複賽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>決賽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一屆</t>
-  </si>
-  <si>
-    <t>歷屆資訊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第二屆</t>
-  </si>
-  <si>
-    <t>第三屆</t>
-  </si>
-  <si>
-    <t>第四屆</t>
-  </si>
-  <si>
-    <t>第五屆</t>
-  </si>
-  <si>
-    <t>第六屆</t>
-  </si>
-  <si>
-    <t>第七屆</t>
-  </si>
-  <si>
-    <t>第八屆</t>
-  </si>
-  <si>
-    <t>第九屆</t>
-  </si>
-  <si>
-    <t>第十屆</t>
-  </si>
-  <si>
-    <t>第十一屆</t>
-  </si>
-  <si>
-    <t>第十二屆</t>
-  </si>
-  <si>
-    <t>第十三屆</t>
-  </si>
-  <si>
-    <t>關於競賽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>留言板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>媒體報導</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>網站架構</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>進入報名網站</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>複賽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HOME&amp;NEWS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>協辦單位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>贊助單位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初賽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>歷屆資訊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注意事項</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>報名資訊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教師研習營</t>
-  </si>
-  <si>
-    <t>學校推廣說明會</t>
-  </si>
-  <si>
-    <t>官方說明會</t>
-  </si>
-  <si>
-    <t>相關活動</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>培訓計畫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>時間與場地</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一梯初賽晉級名單</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大事紀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>競賽歷史</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>競賽理念</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第二梯初賽晉級名單</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>其他</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文宣品</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>電子報</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q&amp;A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>常見問題</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>點我進入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>常用表格</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初賽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>辦法與繳費</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>報名流程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>組隊辦法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>緣起</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>競賽介紹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>組隊辦法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>報名網站</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>常用表格</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大會獎項</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>複賽企業獎</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>決賽企業獎</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初賽時程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>複賽晉級名單</t>
+    <t>進入報名網站</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -449,7 +440,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -475,13 +466,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -519,6 +519,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -804,7 +807,7 @@
   <dimension ref="A2:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5"/>
@@ -815,10 +818,10 @@
   <sheetData>
     <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>0</v>
@@ -833,79 +836,73 @@
         <v>5</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="S3" s="1"/>
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="11" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="11" t="s">
@@ -913,7 +910,7 @@
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="12" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="12" t="s">
@@ -921,25 +918,25 @@
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="11" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="11" t="s">
@@ -947,7 +944,7 @@
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="11" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="12" t="s">
@@ -956,61 +953,64 @@
       <c r="N5" s="2"/>
       <c r="O5" s="1"/>
       <c r="P5" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="6" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="K6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>87</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="11" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="T6" s="2"/>
     </row>
     <row r="7" spans="1:20">
+      <c r="A7" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="11" t="s">
@@ -1018,20 +1018,20 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="10" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M7" s="12" t="s">
         <v>16</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="11" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1041,10 +1041,10 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>11</v>
@@ -1055,17 +1055,17 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="C9" s="1"/>
       <c r="D9" s="11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="11" t="s">
@@ -1074,23 +1074,23 @@
       <c r="I9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="C10" s="1"/>
       <c r="D10" s="11" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>3</v>
@@ -1101,18 +1101,18 @@
       <c r="I10" s="2"/>
       <c r="L10" s="1"/>
       <c r="M10" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="11" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="12" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="11" t="s">
@@ -1120,64 +1120,64 @@
       </c>
       <c r="I11" s="2"/>
       <c r="L11" s="10" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="E12" s="1"/>
       <c r="F12" s="12" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="11" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="O13" s="5"/>
       <c r="P13" s="11" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="O14" s="5"/>
       <c r="P14" s="11" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="7"/>
       <c r="B15" s="8" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="O15" s="5"/>
       <c r="P15" s="11" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="9" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>